<commit_message>
Update triangle board to put LED centroid at footprint origin
</commit_message>
<xml_diff>
--- a/triangle/JLCSMT_BOM.xlsx
+++ b/triangle/JLCSMT_BOM.xlsx
@@ -20,58 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t xml:space="preserve">Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Designator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Footprint</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">LCSC Part #</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">optional</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">）</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">100nF</t>
   </si>
@@ -104,7 +53,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -128,33 +77,19 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -198,20 +133,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -235,7 +166,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8828125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -246,48 +177,35 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>